<commit_message>
FEAT: Add time series extractor almost complete
</commit_message>
<xml_diff>
--- a/tests/data/source_0.xlsx
+++ b/tests/data/source_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ghost\Desktop\cronus-eater\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CA91F5-D036-4321-B36D-37018526F52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C2A4C0-C00C-4597-A89E-96B87ADDCC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7410" yWindow="975" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -383,8 +383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,6 +1029,9 @@
       <c r="J25">
         <v>41</v>
       </c>
+      <c r="L25">
+        <v>23</v>
+      </c>
       <c r="P25" t="s">
         <v>1</v>
       </c>

</xml_diff>